<commit_message>
add supplier speed limiters
</commit_message>
<xml_diff>
--- a/tutorial/supply/tests/supplier_excel_data/限速器缓冲器数据表.xlsx
+++ b/tutorial/supply/tests/supplier_excel_data/限速器缓冲器数据表.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengzhenbo/Library/Mobile Documents/com~apple~CloudDocs/04Project/ElevatorCertificate/ElevatorCertificate/tutorial/supply/供应商数据表/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengzhenbo/Library/Mobile Documents/com~apple~CloudDocs/04Project/ElevatorCertificate/ElevatorCertificate/tutorial/supply/tests/supplier_excel_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804AE480-AB1A-D140-9043-C5A560555CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E294EE4-61BA-FA41-9B17-0A66BD7BE3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="2360" windowWidth="27840" windowHeight="16940" xr2:uid="{B1DEFC15-6C02-1446-A96A-B4848C9C7509}"/>
+    <workbookView xWindow="9100" yWindow="2620" windowWidth="27840" windowHeight="16940" xr2:uid="{B1DEFC15-6C02-1446-A96A-B4848C9C7509}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>序号</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -123,17 +123,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>1998.7.1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2019.03.7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>XZPBK10020290rt</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -143,6 +136,50 @@
   </si>
   <si>
     <t>6k</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>东方</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>x1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bk789</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bk790</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021/3/21</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>x2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2x</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021/3/28</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -766,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063C2400-1601-B34C-86DC-405DF66004D1}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -914,7 +951,7 @@
         <v>21</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I3" s="5">
         <v>5</v>
@@ -923,29 +960,55 @@
         <v>6</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="M3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5" t="s">
-        <v>24</v>
+      <c r="N3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -953,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
@@ -961,7 +1024,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>

</xml_diff>